<commit_message>
Update project untuk branch sorting
</commit_message>
<xml_diff>
--- a/evaluators/dataset_sorting.xlsx
+++ b/evaluators/dataset_sorting.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Punya Orang\OKA\Kuli-ah\skripsi\new\evaluators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50600AD6-0926-4A7E-96FE-F62D60E415D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D2785B-A5BC-4117-A518-3A6FF4F776CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="11625" xr2:uid="{3D9DA0B6-826C-439E-9C93-125696AA4C24}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{3D9DA0B6-826C-439E-9C93-125696AA4C24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1414,8 +1415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC51C9D5-2E9E-42BB-8962-2BFD719F9241}">
   <dimension ref="A1:E325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B246" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C256" sqref="C256"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,7 +1445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>

</xml_diff>